<commit_message>
max pressure first implementation
</commit_message>
<xml_diff>
--- a/coordinatedalgorithms.xlsx
+++ b/coordinatedalgorithms.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Implementations\Mosas Studies\CoordinatedTrafficControlAlgorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE1C0AD5-5937-4F13-9A63-91CA8AD9575E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B24D23-A69E-4A79-AE22-8961BB3AAE6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B799F520-5209-4C24-A23B-39541E2D1861}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8880" xr2:uid="{B799F520-5209-4C24-A23B-39541E2D1861}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>Yöntem</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>52.8 saniye</t>
+  </si>
+  <si>
+    <t>46.6 saniye</t>
   </si>
 </sst>
 </file>
@@ -198,7 +201,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -716,7 +719,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -819,7 +822,9 @@
       <c r="C5" s="5">
         <v>1078</v>
       </c>
-      <c r="D5" s="5"/>
+      <c r="D5" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="E5" s="5"/>
       <c r="F5" s="6"/>
     </row>

</xml_diff>